<commit_message>
printLayout master data reformatted
</commit_message>
<xml_diff>
--- a/scripts/print_layout/printLayout.xlsx
+++ b/scripts/print_layout/printLayout.xlsx
@@ -51,6 +51,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E24C1C-1B4A-4AD5-BFE9-165C7C146AEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -106,6 +156,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C03B67E8-030E-47F2-87C4-A7999AB940D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -161,6 +261,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D9BF43-293F-4575-9470-B3DB84B233B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -216,6 +366,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88BB1C52-5646-45F9-86FE-D654F945182F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -271,6 +471,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5A927FC-F177-43A0-B457-41EBCD294EF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -326,6 +576,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D8EB47-1F8D-416E-BE29-25F6C2B408AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -381,6 +681,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEBB126B-30E3-49C6-A6C0-1AEB89A348D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -436,6 +786,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C16CCE-DBE5-4F7C-B878-271CAD9A948E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -460,6 +860,56 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{775E4517-F5EB-4180-AAB9-A41FEDCE4592}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="9525"/>
+          <a:ext cx="2971800" cy="839856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB321854-1E0B-4915-BDB5-1FD5C9F066E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -512,51 +962,51 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3067D086-92A3-4C30-90AF-135228E663BC}" name="tbl_imdb34" displayName="tbl_imdb34" ref="A3:H4" totalsRowShown="0" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3067D086-92A3-4C30-90AF-135228E663BC}" name="tbl_imdb34" displayName="tbl_imdb34" ref="A3:H4" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5FAA80CA-2402-4236-BDC0-3CF5294CC5BB}" name="ID" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{9E69064A-49B6-42BF-A92B-70665EB7A794}" name="siteName" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{EFD94993-2AB1-44F9-815B-0C520BE096D4}" name="url" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{5CBB2B89-AAFC-4FA1-B156-4CF4B7FE5DEF}" name="username" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{05E047C3-F33A-48E9-A053-7625072852BA}" name="email" dataDxfId="73" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{F4F44BE2-AC6A-4240-8A7F-51395A53C23A}" name="password" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{CD7D49ED-A47E-40CD-AAD0-C54ED2CB4928}" name="changeDate" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{909EB238-0DEA-492C-B9F8-6B3EC84E364E}" name="category" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{5FAA80CA-2402-4236-BDC0-3CF5294CC5BB}" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{9E69064A-49B6-42BF-A92B-70665EB7A794}" name="siteName" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{EFD94993-2AB1-44F9-815B-0C520BE096D4}" name="url" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5CBB2B89-AAFC-4FA1-B156-4CF4B7FE5DEF}" name="username" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{05E047C3-F33A-48E9-A053-7625072852BA}" name="email" dataDxfId="3" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{F4F44BE2-AC6A-4240-8A7F-51395A53C23A}" name="password" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{CD7D49ED-A47E-40CD-AAD0-C54ED2CB4928}" name="changeDate" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{909EB238-0DEA-492C-B9F8-6B3EC84E364E}" name="category" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{009BEF15-4472-4F7A-BE3E-8793FA653383}" name="tbl_imdb349" displayName="tbl_imdb349" ref="A3:H4" totalsRowShown="0" dataDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{009BEF15-4472-4F7A-BE3E-8793FA653383}" name="tbl_imdb349" displayName="tbl_imdb349" ref="A3:H4" totalsRowShown="0" dataDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{89BA219F-D0E9-46EC-8303-497E2FB0761B}" name="ID" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{D8654818-5176-4D50-8AC2-A3D765D6F9EA}" name="siteName" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{619406E0-66EF-439D-B79B-CF7623087C9A}" name="url" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{FC78FD96-3521-4BDD-9396-073CB20638E3}" name="username" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{215AA2E4-45AF-4F0A-896E-3C4211774D01}" name="email" dataDxfId="23" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{B16F4E0C-8D2F-4A04-942F-E6C3F808D23A}" name="password" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{EB16BC7D-C8C0-43D2-9B2C-526160220CBB}" name="changeDate" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{056C2A86-5CC9-4A18-8AB7-79A88499C654}" name="category" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{89BA219F-D0E9-46EC-8303-497E2FB0761B}" name="ID" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{D8654818-5176-4D50-8AC2-A3D765D6F9EA}" name="siteName" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{619406E0-66EF-439D-B79B-CF7623087C9A}" name="url" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{FC78FD96-3521-4BDD-9396-073CB20638E3}" name="username" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{215AA2E4-45AF-4F0A-896E-3C4211774D01}" name="email" dataDxfId="83" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{B16F4E0C-8D2F-4A04-942F-E6C3F808D23A}" name="password" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{EB16BC7D-C8C0-43D2-9B2C-526160220CBB}" name="changeDate" dataDxfId="81"/>
+    <tableColumn id="9" xr3:uid="{056C2A86-5CC9-4A18-8AB7-79A88499C654}" name="category" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{17ADC597-9AC6-430C-94CD-D3FBD24A6829}" name="tbl_imdb347" displayName="tbl_imdb347" ref="A3:H4" totalsRowShown="0" dataDxfId="49" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{17ADC597-9AC6-430C-94CD-D3FBD24A6829}" name="tbl_imdb347" displayName="tbl_imdb347" ref="A3:H4" totalsRowShown="0" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2A6FC618-D764-4DC5-9498-FAB25026E0A2}" name="ID" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{2D89037A-E2CA-4916-911B-9DA896741919}" name="siteName" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{85483621-B60A-4AB5-9278-9F297FF30385}" name="url" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{C000824C-9CB3-4C5F-9439-FF51F3E4A0E5}" name="username" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{C9198A1D-B36F-45C7-B780-C9658CE692F2}" name="email" dataDxfId="43" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{6DA4C6C7-62DD-457F-9AAD-AAB82A7C40B3}" name="password" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{8090E8C4-6324-41A7-A6C3-87A23CBA1469}" name="changeDate" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{7F3E5469-0486-4AF1-8304-0BE6C756191E}" name="category" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{2A6FC618-D764-4DC5-9498-FAB25026E0A2}" name="ID" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{2D89037A-E2CA-4916-911B-9DA896741919}" name="siteName" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{85483621-B60A-4AB5-9278-9F297FF30385}" name="url" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{C000824C-9CB3-4C5F-9439-FF51F3E4A0E5}" name="username" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{C9198A1D-B36F-45C7-B780-C9658CE692F2}" name="email" dataDxfId="73" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{6DA4C6C7-62DD-457F-9AAD-AAB82A7C40B3}" name="password" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{8090E8C4-6324-41A7-A6C3-87A23CBA1469}" name="changeDate" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{7F3E5469-0486-4AF1-8304-0BE6C756191E}" name="category" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,85 +1030,85 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7ECBC457-D3AC-41A0-8A0F-129A89F470CD}" name="tbl_imdb3" displayName="tbl_imdb3" ref="A3:H4" totalsRowShown="0" dataDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7ECBC457-D3AC-41A0-8A0F-129A89F470CD}" name="tbl_imdb3" displayName="tbl_imdb3" ref="A3:H4" totalsRowShown="0" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7F7AB76-DE7F-4885-B391-38B2F227B95A}" name="ID" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{E1EAF7AE-E77C-4D5F-B368-054EE5BEB285}" name="siteName" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{7F90D254-693D-4153-9A24-8E58C0FC7238}" name="url" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{344F0A92-38B9-4F98-8DF4-E05B1510B070}" name="username" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{925455BC-CE21-4F81-B2EC-D481F48BE200}" name="email" dataDxfId="83" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{57C999CE-C629-49EB-B861-B111F9CABCAA}" name="password" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{39B80230-2319-4FC3-B380-83496107E6A2}" name="changeDate" dataDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{679B1402-8135-4A1A-B336-EE285824DCF7}" name="category" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{B7F7AB76-DE7F-4885-B391-38B2F227B95A}" name="ID" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{E1EAF7AE-E77C-4D5F-B368-054EE5BEB285}" name="siteName" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{7F90D254-693D-4153-9A24-8E58C0FC7238}" name="url" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{344F0A92-38B9-4F98-8DF4-E05B1510B070}" name="username" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{925455BC-CE21-4F81-B2EC-D481F48BE200}" name="email" dataDxfId="53" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{57C999CE-C629-49EB-B861-B111F9CABCAA}" name="password" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{39B80230-2319-4FC3-B380-83496107E6A2}" name="changeDate" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{679B1402-8135-4A1A-B336-EE285824DCF7}" name="category" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FF170C42-A1B0-48A3-9A6C-F63BA8CD924B}" name="tbl_imdb3456" displayName="tbl_imdb3456" ref="A3:H4" totalsRowShown="0" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FF170C42-A1B0-48A3-9A6C-F63BA8CD924B}" name="tbl_imdb3456" displayName="tbl_imdb3456" ref="A3:H4" totalsRowShown="0" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C76CE9BE-C822-4458-A321-FD0790EBACE4}" name="ID" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{B0BE6E95-E412-454E-BDBA-520450C5E6F4}" name="siteName" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{6EC44038-B302-4788-8D81-25AB66FA97BF}" name="url" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{BA2826C6-79A7-49C2-99BB-64B097D6CAA9}" name="username" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{9AE8DC5E-9B54-4B1C-8201-BCE1FD0A0A6C}" name="email" dataDxfId="53" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{99132D68-7C9F-4368-9A70-826308ECDAA9}" name="password" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{1FC7B578-F2DC-464D-8A60-43E965BD7423}" name="changeDate" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{A7AFB070-7F0D-4B44-8EC4-C8823416CA43}" name="category" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{C76CE9BE-C822-4458-A321-FD0790EBACE4}" name="ID" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{B0BE6E95-E412-454E-BDBA-520450C5E6F4}" name="siteName" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{6EC44038-B302-4788-8D81-25AB66FA97BF}" name="url" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{BA2826C6-79A7-49C2-99BB-64B097D6CAA9}" name="username" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{9AE8DC5E-9B54-4B1C-8201-BCE1FD0A0A6C}" name="email" dataDxfId="43" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{99132D68-7C9F-4368-9A70-826308ECDAA9}" name="password" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{1FC7B578-F2DC-464D-8A60-43E965BD7423}" name="changeDate" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{A7AFB070-7F0D-4B44-8EC4-C8823416CA43}" name="category" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2A7D6B54-5331-49E5-809E-98A321DEF268}" name="tbl_imdb34911" displayName="tbl_imdb34911" ref="A3:H4" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2A7D6B54-5331-49E5-809E-98A321DEF268}" name="tbl_imdb34911" displayName="tbl_imdb34911" ref="A3:H4" totalsRowShown="0" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{95D9F176-F2E8-47BA-93C8-F85E2D5A3B38}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6C2822A3-9288-4653-8FD8-DD4120D39F8E}" name="siteName" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E67D7E3A-950C-4267-B177-B394B617A42B}" name="url" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4EDA1F6D-5B48-43EB-9FAA-21CE48CC9DCE}" name="username" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{A2342588-F596-47A2-BD6D-9E3B2DA8CA5B}" name="email" dataDxfId="3" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{17096835-6350-42C7-A33E-501FC0C395A1}" name="password" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{AF9D8798-E475-429C-822D-1EC24D7940E5}" name="changeDate" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{9FCAB445-E50A-4F17-8F98-3CB8CE8AC862}" name="category" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{95D9F176-F2E8-47BA-93C8-F85E2D5A3B38}" name="ID" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{6C2822A3-9288-4653-8FD8-DD4120D39F8E}" name="siteName" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{E67D7E3A-950C-4267-B177-B394B617A42B}" name="url" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4EDA1F6D-5B48-43EB-9FAA-21CE48CC9DCE}" name="username" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{A2342588-F596-47A2-BD6D-9E3B2DA8CA5B}" name="email" dataDxfId="33" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{17096835-6350-42C7-A33E-501FC0C395A1}" name="password" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{AF9D8798-E475-429C-822D-1EC24D7940E5}" name="changeDate" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{9FCAB445-E50A-4F17-8F98-3CB8CE8AC862}" name="category" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D1018E58-3700-4BC3-B75F-3D6C11A6129B}" name="tbl_imdb34910" displayName="tbl_imdb34910" ref="A3:H4" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D1018E58-3700-4BC3-B75F-3D6C11A6129B}" name="tbl_imdb34910" displayName="tbl_imdb34910" ref="A3:H4" totalsRowShown="0" dataDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{DEA7E7FE-C80F-4D57-BFA5-EC4446D2B0C4}" name="ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{FC7F562F-640B-474D-8ED6-B92C1882247F}" name="siteName" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{0C4FBEE9-B963-4F62-A4C0-A701BC676578}" name="url" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{1A30B353-0AAF-49DD-A902-1932C53E0659}" name="username" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{138A083B-F062-4164-B271-BA465508BC83}" name="email" dataDxfId="13" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{086609B3-6348-423C-8DE2-F2BBD2C788AC}" name="password" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{86CA6CC8-C5CF-495D-9035-7BAC4B00C3B4}" name="changeDate" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{4EB63F73-2FFC-4D66-9F4F-F96E11424426}" name="category" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{DEA7E7FE-C80F-4D57-BFA5-EC4446D2B0C4}" name="ID" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{FC7F562F-640B-474D-8ED6-B92C1882247F}" name="siteName" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{0C4FBEE9-B963-4F62-A4C0-A701BC676578}" name="url" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1A30B353-0AAF-49DD-A902-1932C53E0659}" name="username" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{138A083B-F062-4164-B271-BA465508BC83}" name="email" dataDxfId="23" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{086609B3-6348-423C-8DE2-F2BBD2C788AC}" name="password" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{86CA6CC8-C5CF-495D-9035-7BAC4B00C3B4}" name="changeDate" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{4EB63F73-2FFC-4D66-9F4F-F96E11424426}" name="category" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A8C4CFD9-9D55-43BD-ADB8-59A47BF1839D}" name="tbl_imdb3478" displayName="tbl_imdb3478" ref="A3:H4" totalsRowShown="0" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A8C4CFD9-9D55-43BD-ADB8-59A47BF1839D}" name="tbl_imdb3478" displayName="tbl_imdb3478" ref="A3:H4" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A3:H4" xr:uid="{B959EE5B-81C3-4ED2-8275-F94600B76136}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1BB7DB47-2076-4438-9BB6-3F2D674DC2BD}" name="ID" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{403ED48B-1E4D-4118-985F-B36753013583}" name="siteName" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{04125361-A59B-45E0-B5FC-1FB4B7FB1A17}" name="url" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{0EE84E4F-38FE-4EB6-9419-3955F1E1997A}" name="username" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{AECD567E-DFB7-40A9-84AC-610395783D71}" name="email" dataDxfId="33" dataCellStyle="Link"/>
-    <tableColumn id="6" xr3:uid="{5CFECA34-CFF2-4854-AAA2-DC1E28E83FF8}" name="password" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{34DF3B8F-903F-467D-B3CD-1244E1F146DF}" name="changeDate" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{F7E610B6-7FD0-4403-BB22-04D771928103}" name="category" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{1BB7DB47-2076-4438-9BB6-3F2D674DC2BD}" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{403ED48B-1E4D-4118-985F-B36753013583}" name="siteName" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{04125361-A59B-45E0-B5FC-1FB4B7FB1A17}" name="url" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{0EE84E4F-38FE-4EB6-9419-3955F1E1997A}" name="username" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{AECD567E-DFB7-40A9-84AC-610395783D71}" name="email" dataDxfId="13" dataCellStyle="Link"/>
+    <tableColumn id="6" xr3:uid="{5CFECA34-CFF2-4854-AAA2-DC1E28E83FF8}" name="password" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{34DF3B8F-903F-467D-B3CD-1244E1F146DF}" name="changeDate" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{F7E610B6-7FD0-4403-BB22-04D771928103}" name="category" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>